<commit_message>
revise measles proportion symptomatic parameters
</commit_message>
<xml_diff>
--- a/gaza_infections/inputs/gaza_infections_parameters.xlsx
+++ b/gaza_infections/inputs/gaza_infections_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Desktop\gaza\gaza_infections\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fchec\Desktop\work\gaza\gaza_infections\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632D639E-A2B6-4CD3-BF42-D6589F34FA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32126A71-2718-4EBC-9EEE-097B3D4D3A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="3" r:id="rId1"/>
@@ -1650,7 +1650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{583212BB-FE43-40DF-83EF-3CBB0F7B7681}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -3542,11 +3542,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{179B2EAC-2BE0-4135-B868-E5A90B2AEFD4}">
   <dimension ref="A1:U124"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D50" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomRight" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5541,7 +5541,7 @@
         <v>15</v>
       </c>
       <c r="F44" s="16">
-        <v>0</v>
+        <v>0.96</v>
       </c>
       <c r="G44" s="17"/>
       <c r="H44" s="17"/>
@@ -5968,7 +5968,7 @@
         <v>15</v>
       </c>
       <c r="F55" s="16">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="G55" s="17"/>
       <c r="H55" s="17"/>

</xml_diff>

<commit_message>
Final version for publication
</commit_message>
<xml_diff>
--- a/gaza_infections/inputs/gaza_infections_parameters.xlsx
+++ b/gaza_infections/inputs/gaza_infections_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fchec\Desktop\work\gaza\gaza_infections\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Desktop\gaza\gaza_infections\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32126A71-2718-4EBC-9EEE-097B3D4D3A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946070D7-5784-4200-9655-A28B55CC0469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="3" r:id="rId1"/>
@@ -1650,8 +1650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{583212BB-FE43-40DF-83EF-3CBB0F7B7681}">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1903,7 +1903,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="4">
-        <v>5000</v>
+        <v>100</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -3542,7 +3542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{179B2EAC-2BE0-4135-B868-E5A90B2AEFD4}">
   <dimension ref="A1:U124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>